<commit_message>
push code, export data into xlsx
</commit_message>
<xml_diff>
--- a/controllers/Expenses01.xlsx
+++ b/controllers/Expenses01.xlsx
@@ -14,21 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="5">
   <si>
-    <t>Rent</t>
+    <t>Prod1</t>
   </si>
   <si>
-    <t>Gas</t>
+    <t>Size</t>
   </si>
   <si>
-    <t>Food</t>
+    <t>L</t>
   </si>
   <si>
-    <t>Gym</t>
+    <t>Prod2</t>
   </si>
   <si>
-    <t>Total</t>
+    <t>All</t>
   </si>
 </sst>
 </file>
@@ -360,51 +360,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="b">
+        <v>0</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="b">
+        <v>0</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="b">
+        <v>0</v>
+      </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="b">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="b">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <f>SUM(B1:B4)</f>
-        <v>0</v>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>